<commit_message>
Inflow_block modified to stage 1
Inflow_blocks modified to enable two-stage modeling
</commit_message>
<xml_diff>
--- a/input_data/input_data_common_start.xlsx
+++ b/input_data/input_data_common_start.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4314D7BF-C374-4070-93B1-D3BE5E28D2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36660FBF-4A3F-4BD3-8FD4-73FEBF29D1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="796" activeTab="1" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" tabRatio="796" activeTab="13" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="timeseries" sheetId="18" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="161">
   <si>
     <t>node</t>
   </si>
@@ -517,6 +517,30 @@
   </si>
   <si>
     <t>ALL</t>
+  </si>
+  <si>
+    <t>b1,dh2</t>
+  </si>
+  <si>
+    <t>b1,s1</t>
+  </si>
+  <si>
+    <t>b1,s2</t>
+  </si>
+  <si>
+    <t>b1,s3</t>
+  </si>
+  <si>
+    <t>b2,dh2</t>
+  </si>
+  <si>
+    <t>b2,s1</t>
+  </si>
+  <si>
+    <t>b2,s2</t>
+  </si>
+  <si>
+    <t>b2,s3</t>
   </si>
 </sst>
 </file>
@@ -900,171 +924,171 @@
   <dimension ref="A1:A49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
     </row>
   </sheetData>
@@ -1080,12 +1104,12 @@
       <selection activeCell="E42" sqref="E42:E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>132</v>
       </c>
@@ -1110,9 +1134,9 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
@@ -1120,7 +1144,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1128,7 +1152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1149,14 +1173,14 @@
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -1174,7 +1198,7 @@
       </c>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -1196,7 +1220,7 @@
       <c r="F2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -1208,15 +1232,15 @@
         <v>0.4</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D25" si="0">1*C3</f>
+        <f t="shared" ref="D3:D6" si="0">1*C3</f>
         <v>0.4</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E25" si="1">1*C3</f>
+        <f t="shared" ref="E3:E6" si="1">1*C3</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -1236,7 +1260,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -1256,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -1276,115 +1300,115 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -1405,14 +1429,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
-    <col min="4" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -1435,7 +1459,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -1463,7 +1487,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -1479,19 +1503,19 @@
         <v>-5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E25" si="0">1*C3</f>
+        <f t="shared" ref="E3:E6" si="0">1*C3</f>
         <v>-5</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F25" si="1">1*B3</f>
+        <f t="shared" ref="F3:F6" si="1">1*B3</f>
         <v>-5</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G25" si="2">1*C3</f>
+        <f t="shared" ref="G3:G6" si="2">1*C3</f>
         <v>-5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -1519,7 +1543,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -1531,7 +1555,7 @@
         <v>-3</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D3:D25" si="3">1*B5</f>
+        <f t="shared" ref="D5:D6" si="3">1*B5</f>
         <v>-2</v>
       </c>
       <c r="E5">
@@ -1547,7 +1571,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -1575,7 +1599,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
@@ -1583,7 +1607,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
@@ -1591,7 +1615,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
@@ -1599,7 +1623,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
@@ -1607,7 +1631,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
@@ -1615,7 +1639,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
@@ -1623,7 +1647,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
@@ -1631,7 +1655,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
@@ -1639,7 +1663,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
@@ -1647,7 +1671,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
@@ -1655,7 +1679,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
@@ -1663,7 +1687,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
@@ -1671,7 +1695,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
@@ -1679,7 +1703,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
@@ -1687,7 +1711,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
@@ -1695,7 +1719,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
@@ -1703,7 +1727,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
@@ -1711,7 +1735,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
@@ -1719,7 +1743,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -1736,88 +1760,135 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098BD40C-3F1E-4DCA-B153-EDE213641CC0}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="7">
+        <v>44671.041666666664</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-2</v>
+      </c>
+      <c r="F2" s="7">
+        <v>44671.124999826388</v>
+      </c>
+      <c r="G2" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>44671.08333321759</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>44671.166666435187</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
+      <c r="B4" s="7">
+        <v>44671.124999826388</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1836,12 +1907,12 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -1849,7 +1920,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -1858,7 +1929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -1867,7 +1938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -1876,7 +1947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -1885,7 +1956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -1894,115 +1965,115 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -2021,17 +2092,17 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -2066,7 +2137,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -2101,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>40</v>
       </c>
@@ -2136,7 +2207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
@@ -2171,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>42</v>
       </c>
@@ -2219,13 +2290,13 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>128</v>
       </c>
@@ -2239,7 +2310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -2253,7 +2324,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
@@ -2267,7 +2338,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>42</v>
       </c>
@@ -2291,17 +2362,17 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
-    <col min="2" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="13" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
+    <col min="2" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -2342,7 +2413,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -2392,7 +2463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -2442,7 +2513,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -2492,7 +2563,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -2534,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -2576,115 +2647,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -2704,14 +2775,14 @@
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="7" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -2734,7 +2805,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -2764,7 +2835,7 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -2794,7 +2865,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -2824,7 +2895,7 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -2854,7 +2925,7 @@
         <v>22.95</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -2884,115 +2955,115 @@
         <v>16.650000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -3008,17 +3079,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82624B08-6930-4D2B-BCBB-C78CE759E704}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -3026,7 +3097,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -3034,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -3042,7 +3113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -3050,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -3058,7 +3129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>145</v>
       </c>
@@ -3066,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -3074,7 +3145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -3096,12 +3167,12 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -3109,7 +3180,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -3117,7 +3188,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -3138,9 +3209,9 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -3148,7 +3219,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -3156,7 +3227,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -3164,7 +3235,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -3185,162 +3256,162 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -3359,12 +3430,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -3378,7 +3449,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -3393,7 +3464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -3408,7 +3479,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -3423,7 +3494,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -3438,7 +3509,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -3453,115 +3524,115 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -3581,14 +3652,14 @@
       <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -3602,7 +3673,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -3616,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -3635,15 +3706,15 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
-    <col min="2" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
+    <col min="2" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -3675,7 +3746,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -3708,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -3741,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -3774,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -3807,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -3840,115 +3911,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -3967,12 +4038,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -3986,7 +4057,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
@@ -4001,7 +4072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
@@ -4016,7 +4087,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
@@ -4031,7 +4102,7 @@
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
@@ -4046,7 +4117,7 @@
         <v>4.4117647058823533</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
@@ -4061,115 +4132,115 @@
         <v>4.5454545454545459</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -4188,20 +4259,20 @@
       <selection activeCell="L12" activeCellId="1" sqref="M1 L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4322,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4301,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4351,7 +4422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4401,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4451,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4501,7 +4572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -4515,7 +4586,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M8" s="6"/>
     </row>
   </sheetData>
@@ -4531,22 +4602,22 @@
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -4599,7 +4670,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4652,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4705,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -4758,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4811,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -4864,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -4917,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -4948,9 +5019,9 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
@@ -4961,7 +5032,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4972,7 +5043,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4983,7 +5054,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -4994,7 +5065,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -5018,9 +5089,9 @@
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -5077,20 +5148,20 @@
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -5122,7 +5193,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -5154,7 +5225,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -5186,7 +5257,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -5218,7 +5289,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -5250,7 +5321,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -5282,7 +5353,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -5314,7 +5385,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
@@ -5346,7 +5417,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -5378,7 +5449,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>81</v>
       </c>
@@ -5410,7 +5481,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
@@ -5442,7 +5513,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5488,155 +5559,155 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>IF(timeseries!A2&lt;&gt;"",timeseries!A2,"")</f>
         <v>44671</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>IF(timeseries!A3&lt;&gt;"",timeseries!A3,"")</f>
         <v>44671.041666666664</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>IF(timeseries!A4&lt;&gt;"",timeseries!A4,"")</f>
         <v>44671.08333321759</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>IF(timeseries!A5&lt;&gt;"",timeseries!A5,"")</f>
         <v>44671.124999826388</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>IF(timeseries!A6&lt;&gt;"",timeseries!A6,"")</f>
         <v>44671.166666435187</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f>IF(timeseries!A7&lt;&gt;"",timeseries!A7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f>IF(timeseries!A8&lt;&gt;"",timeseries!A8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f>IF(timeseries!A9&lt;&gt;"",timeseries!A9,"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f>IF(timeseries!A10&lt;&gt;"",timeseries!A10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f>IF(timeseries!A11&lt;&gt;"",timeseries!A11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f>IF(timeseries!A12&lt;&gt;"",timeseries!A12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f>IF(timeseries!A13&lt;&gt;"",timeseries!A13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f>IF(timeseries!A14&lt;&gt;"",timeseries!A14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f>IF(timeseries!A15&lt;&gt;"",timeseries!A15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f>IF(timeseries!A16&lt;&gt;"",timeseries!A16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f>IF(timeseries!A17&lt;&gt;"",timeseries!A17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f>IF(timeseries!A18&lt;&gt;"",timeseries!A18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f>IF(timeseries!A19&lt;&gt;"",timeseries!A19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f>IF(timeseries!A20&lt;&gt;"",timeseries!A20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f>IF(timeseries!A21&lt;&gt;"",timeseries!A21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f>IF(timeseries!A22&lt;&gt;"",timeseries!A22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f>IF(timeseries!A23&lt;&gt;"",timeseries!A23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f>IF(timeseries!A24&lt;&gt;"",timeseries!A24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f>IF(timeseries!A25&lt;&gt;"",timeseries!A25,"")</f>
         <v/>
@@ -5655,14 +5726,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>132</v>
       </c>

</xml_diff>